<commit_message>
fm10-rev5: Match current part numbers
</commit_message>
<xml_diff>
--- a/fieldmill10/fab/fieldmill10-rev5/BOM-lista.xlsx
+++ b/fieldmill10/fab/fieldmill10-rev5/BOM-lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="203">
   <si>
     <t xml:space="preserve">Gulmarkerad=Tillkommande komponenter</t>
   </si>
@@ -175,63 +175,63 @@
     <t xml:space="preserve">Cap cer 10u</t>
   </si>
   <si>
-    <t xml:space="preserve">±20% 10V X7R soft termination</t>
+    <t xml:space="preserve">±20% 10V X7R soft termination or better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGA4J1X7S1C106K125AE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-173674-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">810-CGA4J1X7S1C106KA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.se/product-detail/en/tdk-corporation/CGA4J1X7S1C106K125AE/445-173674-1-ND/5809745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21 C30 C32 C36 C38 C42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap silver mica 1p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">±0.5pF 100V mica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cornell Dubilier Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC08CA010D-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">338-1339-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5982-08-100V1.0-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.se/product-detail/en/cornell-dubilier-electronics-cde/MC08CA010D-F/338-1339-ND/969296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://se.farnell.com/cornell-dubilier/mc08ca010d-f/capacitor-rf-microwave-1pf-100v/dp/1610819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 C13 C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap cer 1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">±10% 25V X7R soft termination</t>
   </si>
   <si>
     <t xml:space="preserve">KEMET</t>
   </si>
   <si>
-    <t xml:space="preserve">C0805X106M8RACAUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">399-15692-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-C0805X106M8RAUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.se/product-detail/en/kemet/C0805X106M8RACAUTO/399-15692-1-ND/7427572</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://se.farnell.com/kemet/c0805x106m8racauto/cap-mlcc-aec-q200-x7r-20-10v-0805/dp/2776919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21 C30 C32 C36 C38 C42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cap silver mica 1p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">±0.5pF 100V mica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cornell Dubilier Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC08CA010D-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">338-1339-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5982-08-100V1.0-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.se/product-detail/en/cornell-dubilier-electronics-cde/MC08CA010D-F/338-1339-ND/969296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://se.farnell.com/cornell-dubilier/mc08ca010d-f/capacitor-rf-microwave-1pf-100v/dp/1610819</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6 C13 C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cap cer 1u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">±10% 25V X7R soft termination</t>
-  </si>
-  <si>
     <t xml:space="preserve">C0805X105K3RACAUTO</t>
   </si>
   <si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t xml:space="preserve">R11 R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49,9</t>
   </si>
   <si>
     <t xml:space="preserve">U3</t>
@@ -748,7 +751,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,6 +801,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,8 +895,8 @@
   </sheetPr>
   <dimension ref="A1:W65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,7 +1155,7 @@
       <c r="F8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>51</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -1161,28 +1168,24 @@
         <v>30</v>
       </c>
       <c r="K8" s="0"/>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="O8" s="0" t="n">
-        <v>2776919</v>
-      </c>
+      <c r="O8" s="0"/>
       <c r="P8" s="0"/>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="R8" s="0" t="s">
+      <c r="R8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="S8" s="0" t="s">
-        <v>57</v>
-      </c>
+      <c r="S8" s="0"/>
       <c r="T8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,13 +1198,13 @@
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>41</v>
@@ -1214,26 +1217,26 @@
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="N9" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="O9" s="0" t="n">
         <v>1610819</v>
       </c>
       <c r="P9" s="0"/>
       <c r="Q9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="S9" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="S9" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="T9" s="0"/>
     </row>
@@ -1247,13 +1250,13 @@
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="G10" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>41</v>
@@ -1266,7 +1269,7 @@
       </c>
       <c r="K10" s="0"/>
       <c r="L10" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>70</v>
@@ -1433,7 +1436,7 @@
       <c r="O13" s="0" t="n">
         <v>9907874</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="14" t="s">
         <v>99</v>
       </c>
       <c r="Q13" s="0" t="s">
@@ -1460,13 +1463,13 @@
       <c r="E14" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>105</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>105</v>
       </c>
       <c r="I14" s="0" t="s">
@@ -1560,13 +1563,13 @@
       <c r="E16" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="15" t="s">
         <v>120</v>
       </c>
       <c r="I16" s="0" t="s">
@@ -1908,8 +1911,8 @@
       <c r="E24" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F24" s="12" t="n">
-        <v>50</v>
+      <c r="F24" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>139</v>
@@ -1946,16 +1949,16 @@
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>29</v>
@@ -1965,26 +1968,26 @@
       </c>
       <c r="K25" s="0"/>
       <c r="L25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O25" s="0" t="n">
         <v>2580620</v>
       </c>
       <c r="P25" s="0"/>
       <c r="Q25" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T25" s="0"/>
       <c r="U25" s="0"/>
@@ -2000,16 +2003,16 @@
       </c>
       <c r="D26" s="0"/>
       <c r="E26" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>29</v>
@@ -2019,26 +2022,26 @@
       </c>
       <c r="K26" s="0"/>
       <c r="L26" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>2518724</v>
       </c>
       <c r="P26" s="0"/>
       <c r="Q26" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="T26" s="0"/>
       <c r="U26" s="0"/>
@@ -2054,16 +2057,16 @@
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>29</v>
@@ -2076,23 +2079,23 @@
         <v>97</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>2778100</v>
       </c>
       <c r="P27" s="0"/>
       <c r="Q27" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T27" s="0"/>
       <c r="U27" s="0"/>
@@ -2108,16 +2111,16 @@
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>29</v>
@@ -2127,31 +2130,31 @@
       </c>
       <c r="K28" s="0"/>
       <c r="L28" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>2781817</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T28" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U28" s="0"/>
       <c r="V28" s="0"/>
@@ -2166,16 +2169,16 @@
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>29</v>
@@ -2185,21 +2188,21 @@
       </c>
       <c r="K29" s="0"/>
       <c r="L29" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="M29" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="M29" s="0" t="s">
-        <v>182</v>
-      </c>
       <c r="N29" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O29" s="0"/>
       <c r="P29" s="0"/>
       <c r="Q29" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S29" s="0"/>
       <c r="T29" s="0"/>
@@ -2216,16 +2219,16 @@
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>29</v>
@@ -2235,26 +2238,26 @@
       </c>
       <c r="K30" s="0"/>
       <c r="L30" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>2510952</v>
       </c>
       <c r="P30" s="0"/>
       <c r="Q30" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="S30" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T30" s="0"/>
       <c r="U30" s="0"/>
@@ -2270,16 +2273,16 @@
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>29</v>
@@ -2289,26 +2292,26 @@
       </c>
       <c r="K31" s="0"/>
       <c r="L31" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="O31" s="0" t="n">
         <v>2514723</v>
       </c>
       <c r="P31" s="0"/>
       <c r="Q31" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S31" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="T31" s="0"/>
       <c r="U31" s="0"/>

</xml_diff>

<commit_message>
fm10: Remove R8 from fab files
</commit_message>
<xml_diff>
--- a/fieldmill10/fab/fieldmill10-rev5/BOM-lista.xlsx
+++ b/fieldmill10/fab/fieldmill10-rev5/BOM-lista.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Rev 5" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Rev 4.1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="204">
   <si>
     <t xml:space="preserve">Gulmarkerad=Tillkommande komponenter</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">fieldmill10</t>
   </si>
   <si>
+    <t xml:space="preserve">4.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grön markerad = Ändrat komponentvärde</t>
   </si>
   <si>
@@ -400,7 +403,7 @@
     <t xml:space="preserve">R_1206</t>
   </si>
   <si>
-    <t xml:space="preserve">R2 R8 R10 R31 R55 R56</t>
+    <t xml:space="preserve">R2 R10 R31 R55 R56</t>
   </si>
   <si>
     <t xml:space="preserve">R_0805</t>
@@ -678,7 +681,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,7 +697,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF3333"/>
       </patternFill>
     </fill>
     <fill>
@@ -707,6 +710,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
         <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -772,10 +781,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -813,6 +818,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -872,7 +881,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -895,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:W65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -943,93 +952,93 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
-      <c r="P4" s="7"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="L5" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="M5" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="N5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="R5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="S5" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T5" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
@@ -1038,54 +1047,54 @@
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="G6" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="H6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K6" s="0"/>
       <c r="L6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O6" s="0" t="n">
         <v>9695001</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
@@ -1094,54 +1103,54 @@
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>27</v>
+      <c r="F7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K7" s="0"/>
       <c r="L7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>9694897</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="0" t="n">
         <v>3</v>
       </c>
@@ -1150,46 +1159,46 @@
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>51</v>
       </c>
+      <c r="G8" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="H8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K8" s="0"/>
-      <c r="L8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="14" t="s">
+      <c r="L8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="M8" s="13" t="s">
         <v>54</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="O8" s="0"/>
       <c r="P8" s="0"/>
-      <c r="Q8" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="R8" s="14" t="s">
+      <c r="Q8" s="13" t="s">
         <v>56</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="S8" s="0"/>
       <c r="T8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="0" t="n">
         <v>4</v>
       </c>
@@ -1198,50 +1207,50 @@
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="G9" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="H9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O9" s="0" t="n">
         <v>1610819</v>
       </c>
       <c r="P9" s="0"/>
       <c r="Q9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="0" t="n">
         <v>5</v>
       </c>
@@ -1250,50 +1259,50 @@
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>68</v>
       </c>
+      <c r="G10" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="H10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K10" s="0"/>
       <c r="L10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O10" s="0" t="n">
         <v>2478267</v>
       </c>
       <c r="P10" s="0"/>
       <c r="Q10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="T10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="0" t="n">
         <v>6</v>
       </c>
@@ -1302,46 +1311,46 @@
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>77</v>
       </c>
+      <c r="G11" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="H11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K11" s="0"/>
       <c r="L11" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O11" s="0"/>
       <c r="P11" s="0"/>
       <c r="Q11" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S11" s="0"/>
       <c r="T11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="0" t="n">
         <v>7</v>
       </c>
@@ -1350,54 +1359,54 @@
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>85</v>
       </c>
+      <c r="G12" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="H12" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K12" s="0"/>
       <c r="L12" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O12" s="0" t="n">
         <v>1431141</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="0" t="n">
         <v>8</v>
       </c>
@@ -1406,53 +1415,53 @@
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>96</v>
       </c>
+      <c r="G13" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="H13" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K13" s="0"/>
       <c r="L13" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>9907874</v>
       </c>
-      <c r="P13" s="14" t="s">
-        <v>99</v>
+      <c r="P13" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>9</v>
       </c>
@@ -1461,38 +1470,38 @@
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="F14" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>105</v>
+      <c r="G14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K14" s="0"/>
       <c r="L14" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O14" s="0"/>
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
       <c r="R14" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S14" s="0"/>
       <c r="T14" s="0"/>
@@ -1501,7 +1510,7 @@
       <c r="W14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="0" t="n">
         <v>10</v>
       </c>
@@ -1510,40 +1519,40 @@
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>112</v>
       </c>
+      <c r="G15" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="H15" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K15" s="0"/>
       <c r="L15" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O15" s="0"/>
       <c r="P15" s="0"/>
       <c r="Q15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S15" s="0"/>
       <c r="T15" s="0"/>
@@ -1552,7 +1561,7 @@
       <c r="W15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="0" t="n">
         <v>11</v>
       </c>
@@ -1561,38 +1570,38 @@
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>120</v>
+      <c r="F16" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K16" s="0"/>
       <c r="L16" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O16" s="0"/>
       <c r="P16" s="0"/>
       <c r="Q16" s="0"/>
       <c r="R16" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="S16" s="0"/>
       <c r="T16" s="0"/>
@@ -1601,7 +1610,7 @@
       <c r="W16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="0" t="n">
         <v>12</v>
       </c>
@@ -1610,23 +1619,23 @@
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="12" t="n">
+        <v>124</v>
+      </c>
+      <c r="F17" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>124</v>
+      <c r="G17" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J17" s="0"/>
       <c r="K17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
@@ -1642,7 +1651,7 @@
       <c r="W17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="0" t="n">
         <v>13</v>
       </c>
@@ -1650,24 +1659,24 @@
         <v>6</v>
       </c>
       <c r="D18" s="0"/>
-      <c r="E18" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="12" t="n">
+      <c r="E18" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>124</v>
+      <c r="G18" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
@@ -1683,7 +1692,7 @@
       <c r="W18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="0" t="n">
         <v>14</v>
       </c>
@@ -1692,45 +1701,45 @@
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>130</v>
       </c>
+      <c r="G19" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="H19" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K19" s="0"/>
       <c r="L19" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O19" s="0" t="n">
         <v>1109056</v>
       </c>
       <c r="P19" s="0"/>
       <c r="Q19" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="T19" s="0"/>
       <c r="U19" s="0"/>
@@ -1738,7 +1747,7 @@
       <c r="W19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="0" t="n">
         <v>15</v>
       </c>
@@ -1747,23 +1756,23 @@
       </c>
       <c r="D20" s="0"/>
       <c r="E20" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>139</v>
       </c>
+      <c r="G20" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="H20" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J20" s="0"/>
       <c r="K20" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
@@ -1779,7 +1788,7 @@
       <c r="W20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="0" t="n">
         <v>16</v>
       </c>
@@ -1788,23 +1797,23 @@
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="H21" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J21" s="0"/>
       <c r="K21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
@@ -1820,7 +1829,7 @@
       <c r="W21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="0" t="n">
         <v>17</v>
       </c>
@@ -1829,23 +1838,23 @@
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F22" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>139</v>
+      <c r="F22" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J22" s="0"/>
       <c r="K22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
@@ -1869,23 +1878,23 @@
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>139</v>
+      <c r="F23" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J23" s="0"/>
       <c r="K23" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
@@ -1909,23 +1918,23 @@
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>139</v>
+      <c r="F24" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J24" s="0"/>
       <c r="K24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
@@ -1949,45 +1958,45 @@
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="F25" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>150</v>
       </c>
+      <c r="G25" s="11" t="s">
+        <v>151</v>
+      </c>
       <c r="H25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K25" s="0"/>
       <c r="L25" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O25" s="0" t="n">
         <v>2580620</v>
       </c>
       <c r="P25" s="0"/>
       <c r="Q25" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="T25" s="0"/>
       <c r="U25" s="0"/>
@@ -2003,45 +2012,45 @@
       </c>
       <c r="D26" s="0"/>
       <c r="E26" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>159</v>
       </c>
+      <c r="G26" s="11" t="s">
+        <v>160</v>
+      </c>
       <c r="H26" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K26" s="0"/>
       <c r="L26" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>2518724</v>
       </c>
       <c r="P26" s="0"/>
       <c r="Q26" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T26" s="0"/>
       <c r="U26" s="0"/>
@@ -2057,45 +2066,45 @@
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>168</v>
       </c>
+      <c r="G27" s="11" t="s">
+        <v>169</v>
+      </c>
       <c r="H27" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K27" s="0"/>
       <c r="L27" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>2778100</v>
       </c>
       <c r="P27" s="0"/>
       <c r="Q27" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T27" s="0"/>
       <c r="U27" s="0"/>
@@ -2111,50 +2120,50 @@
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="F28" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>150</v>
+      <c r="F28" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K28" s="0"/>
       <c r="L28" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>2781817</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="T28" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U28" s="0"/>
       <c r="V28" s="0"/>
@@ -2169,40 +2178,40 @@
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="F29" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>150</v>
+      <c r="F29" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K29" s="0"/>
       <c r="L29" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="M29" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="M29" s="0" t="s">
-        <v>183</v>
-      </c>
       <c r="N29" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O29" s="0"/>
       <c r="P29" s="0"/>
       <c r="Q29" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S29" s="0"/>
       <c r="T29" s="0"/>
@@ -2219,45 +2228,45 @@
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="F30" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>168</v>
+      <c r="F30" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K30" s="0"/>
       <c r="L30" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>2510952</v>
       </c>
       <c r="P30" s="0"/>
       <c r="Q30" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S30" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T30" s="0"/>
       <c r="U30" s="0"/>
@@ -2273,45 +2282,45 @@
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>197</v>
       </c>
+      <c r="G31" s="11" t="s">
+        <v>198</v>
+      </c>
       <c r="H31" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K31" s="0"/>
       <c r="L31" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="O31" s="0" t="n">
         <v>2514723</v>
       </c>
       <c r="P31" s="0"/>
       <c r="Q31" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="S31" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="T31" s="0"/>
       <c r="U31" s="0"/>

</xml_diff>